<commit_message>
Minor changes in geos data file
</commit_message>
<xml_diff>
--- a/8-data-visualization/geos.xlsx
+++ b/8-data-visualization/geos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonqo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonqo\Git\msc-data-science\8-data-visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAE8628-4EF5-483A-A1CB-50A19E37B22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D74828-819F-4636-A673-BFB332BD3F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
@@ -20,15 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t>AT] Austria</t>
+  </si>
+  <si>
+    <t>[FX] Non metropolitan France</t>
+  </si>
+  <si>
+    <t>geo</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[EU27_2020] European Union - 27 countries (from 2020)</t>
@@ -40,8 +49,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[EU28] European Union - 28 countries (2013-2020)</t>
@@ -53,8 +62,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[BE] Belgium</t>
@@ -66,8 +75,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[BG] Bulgaria</t>
@@ -79,8 +88,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[CZ] Czechia</t>
@@ -92,8 +101,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[DK] Denmark</t>
@@ -105,8 +114,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[DE] Germany (until 1990 former territory of the FRG)</t>
@@ -118,8 +127,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[EE] Estonia</t>
@@ -131,8 +140,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[IE] Ireland</t>
@@ -144,8 +153,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[EL] Greece</t>
@@ -157,8 +166,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[ES] Spain</t>
@@ -170,8 +179,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[FR] France</t>
@@ -183,8 +192,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[HR] Croatia</t>
@@ -196,8 +205,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[IT] Italy</t>
@@ -209,8 +218,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[CY] Cyprus</t>
@@ -222,8 +231,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[LV] Latvia</t>
@@ -235,8 +244,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[LT] Lithuania</t>
@@ -248,8 +257,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[LU] Luxembourg</t>
@@ -261,8 +270,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[HU] Hungary</t>
@@ -274,8 +283,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[MT] Malta</t>
@@ -287,24 +296,21 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[NL] Netherlands</t>
     </r>
   </si>
   <si>
-    <t>AT] Austria</t>
-  </si>
-  <si>
-    <r>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[PL] Poland</t>
@@ -316,8 +322,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[PT] Portugal</t>
@@ -329,8 +335,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[RO] Romania</t>
@@ -342,8 +348,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[SI] Slovenia</t>
@@ -355,8 +361,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[SK] Slovakia</t>
@@ -368,8 +374,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[FI] Finland</t>
@@ -381,8 +387,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[SE] Sweden</t>
@@ -394,8 +400,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[IS] Iceland</t>
@@ -407,8 +413,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[LI] Liechtenstein</t>
@@ -420,8 +426,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[NO] Norway</t>
@@ -433,8 +439,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[CH] Switzerland</t>
@@ -446,8 +452,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[UK] United Kingdom</t>
@@ -459,8 +465,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[RS] Serbia</t>
@@ -472,22 +478,19 @@
     </r>
     <r>
       <rPr>
-        <sz val="8"/>
-        <color rgb="FF212121"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
       <t>[TR] Türkiye</t>
     </r>
-  </si>
-  <si>
-    <t>[FX] Non metropolitan France</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,18 +644,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF212121"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212121"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,12 +827,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0E0E0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -999,17 +990,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1066,6 +1048,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{905582B8-91FC-4E58-BA62-2CA0CBE9D271}" name="Table3" displayName="Table3" ref="A1:A1048576" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:A1048576" xr:uid="{905582B8-91FC-4E58-BA62-2CA0CBE9D271}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{5BB95A5E-F8FF-424E-A4C1-CE5E33D69870}" name="geo" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1365,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" customHeight="1"/>
@@ -1377,192 +1369,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="24" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.6" customHeight="1">
+      <c r="A38" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.6" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>